<commit_message>
Add qualitative comparison figure generation and docs
Introduced QUALITATIVE_COMPARISON_USAGE.md with detailed usage instructions for generating qualitative comparison figures. Enhanced generate_qualitative_comparison.py with argparse CLI, reproducible random seed support, improved output, and JSON metadata export. Updated README.md to clarify output directories and checkpoint handling. Added new qualitative comparison figures, metadata, and batch scripts; removed move_models_to_runs.py and reorganized scripts for clarity.
</commit_message>
<xml_diff>
--- a/results/CIFAR10/simplecnn/noise_0.0/Momentum/runs_and_aggregate.xlsx
+++ b/results/CIFAR10/simplecnn/noise_0.0/Momentum/runs_and_aggregate.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="aggregate" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="run_1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="run_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="run_3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="run_4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="run_5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="aggregate" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>